<commit_message>
added files palas/excel for clean main file
</commit_message>
<xml_diff>
--- a/palas.xlsx
+++ b/palas.xlsx
@@ -644,56 +644,56 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SIUX VIKING III</t>
+          <t>RS COBRA EDITION NEGRO NARANJA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SKU: 24756-P</t>
+          <t>SKU: 28442-P</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>44,95 €</t>
+          <t>46,95 €</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-viking-iii-24756-p</t>
+          <t>https://www.padelnuestro.com/rs-cobra-edition-negro-naranja-28442-p</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RS COBRA EDITION NEGRO NARANJA</t>
+          <t>SOFTEE RANGER ORANGE 2024</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SKU: 28442-P</t>
+          <t>SKU: 112481-P</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>46,95 €</t>
+          <t>47,95 €</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/rs-cobra-edition-negro-naranja-28442-p</t>
+          <t>https://www.padelnuestro.com/softee-ranger-orange-2024-112481-p</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SOFTEE RANGER ORANGE 2024</t>
+          <t>WILSON PRO STAFF V2 TEAM NEGRO ROJO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SKU: 112481-P</t>
+          <t>SKU: 27960-P</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -703,19 +703,19 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/softee-ranger-orange-2024-112481-p</t>
+          <t>https://www.padelnuestro.com/wilson-pro-staff-v2-team-negro-rojo-27960-p</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>WILSON PRO STAFF V2 TEAM NEGRO ROJO</t>
+          <t>WILSON BLADE TEAM V2 BLACK</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SKU: 27960-P</t>
+          <t>SKU: 27951-P</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -725,41 +725,41 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/wilson-pro-staff-v2-team-negro-rojo-27960-p</t>
+          <t>https://www.padelnuestro.com/wilson-blade-team-v2-black-27951-p</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>WILSON BLADE TEAM V2 BLACK</t>
+          <t>PALA SIUX SX7</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SKU: 27951-P</t>
+          <t>SKU: 28785-P</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>47,95 €</t>
+          <t>49,95 €</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/wilson-blade-team-v2-black-27951-p</t>
+          <t>https://www.padelnuestro.com/pala-siux-sx7-28785-p</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SOFTEE PRO MASTER EVOLUTION NARANJA</t>
+          <t>DUNLOP IMPACT HL RED</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SKU: 30968-P</t>
+          <t>SKU: 29699-P</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -769,19 +769,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/softee-pro-master-evolution-naranja-30968-p</t>
+          <t>https://www.padelnuestro.com/dunlop-impact-hl-red-29699-p</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DUNLOP RENEGADE SOFT</t>
+          <t>SOFTEE PRO MASTER EVOLUTION AMARILLO</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SKU: 21583-P</t>
+          <t>SKU: 30966-P</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -791,19 +791,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-renegade-soft-21583-p</t>
+          <t>https://www.padelnuestro.com/softee-pro-master-evolution-amarillo-30966-p</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DUNLOP IMPACT HL RED</t>
+          <t>SOFTEE PRO MASTER EVOLUTION NARANJA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SKU: 29699-P</t>
+          <t>SKU: 30968-P</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -813,19 +813,19 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-impact-hl-red-29699-p</t>
+          <t>https://www.padelnuestro.com/softee-pro-master-evolution-naranja-30968-p</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SOFTEE PRO MASTER EVOLUTION AMARILLO</t>
+          <t>PICKLEBALL HEAD EXTREME ELITE 2023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SKU: 30966-P</t>
+          <t>SKU: 108823-P</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -835,19 +835,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/softee-pro-master-evolution-amarillo-30966-p</t>
+          <t>https://www.padelnuestro.com/pickleball-head-extreme-elite-2023-108823-p</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PALA SIUX SX7</t>
+          <t>WILSON PRO STAFF V2 TEAM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SKU: 28785-P</t>
+          <t>SKU: 27961-P</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -857,19 +857,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/pala-siux-sx7-28785-p</t>
+          <t>https://www.padelnuestro.com/wilson-pro-staff-v2-team-27961-p</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>WILSON PRO STAFF V2 TEAM</t>
+          <t>HEAD SPEED JUNIOR 2023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SKU: 27961-P</t>
+          <t>SKU: 32522-P</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -879,107 +879,107 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/wilson-pro-staff-v2-team-27961-p</t>
+          <t>https://www.padelnuestro.com/head-speed-junior-2023-32522-p</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PICKLEBALL HEAD EXTREME ELITE 2023</t>
+          <t>DUNLOP ROCKET TOUR AZUL</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SKU: 108823-P</t>
+          <t>SKU: 104760-P</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>49,95 €</t>
+          <t>50,95 €</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/pickleball-head-extreme-elite-2023-108823-p</t>
+          <t>https://www.padelnuestro.com/dunlop-rocket-tour-azul-104760-p</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>HEAD SPEED JUNIOR 2023</t>
+          <t>BLACK CROWN PITON JUNIOR</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SKU: 32522-P</t>
+          <t>SKU: 6006-P</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>49,95 €</t>
+          <t>50,95 €</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-speed-junior-2023-32522-p</t>
+          <t>https://www.padelnuestro.com/black-crown-piton-junior-6006-p</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DUNLOP ROCKET TOUR AZUL</t>
+          <t>J.HAYBER WARRIOR FIT</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SKU: 104760-P</t>
+          <t>SKU: 23627-P</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>50,95 €</t>
+          <t>51,95 €</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-rocket-tour-azul-104760-p</t>
+          <t>https://www.padelnuestro.com/j-hayber-warrior-fit-23627-p</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BLACK CROWN PITON JUNIOR</t>
+          <t>BULLPADEL INDIGA PWR 2024</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SKU: 6006-P</t>
+          <t>SKU: 32437-P</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>50,95 €</t>
+          <t>51,95 €</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-piton-junior-6006-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-indiga-pwr-2024-32437-p</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>J.HAYBER WARRIOR FIT</t>
+          <t>VAIRO ACROSS BLUE</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SKU: 23627-P</t>
+          <t>SKU: 105769-P</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -989,19 +989,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/j-hayber-warrior-fit-23627-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-blue-105769-p</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS BLUE</t>
+          <t>ADIDAS DRIVE 3.3 BLUE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SKU: 105769-P</t>
+          <t>SKU: 110135-P</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1011,41 +1011,41 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-blue-105769-p</t>
+          <t>https://www.padelnuestro.com/adidas-drive-3-3-blue-110135-p</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ADIDAS DRIVE 3.3 BLUE</t>
+          <t>BULLPADEL INDIGA W MUJER 2023</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SKU: 110135-P</t>
+          <t>SKU: 32439-P</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>51,95 €</t>
+          <t>52,95 €</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-drive-3-3-blue-110135-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-indiga-w-mujer-2023-32439-p</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BULLPADEL INDIGA W MUJER 2023</t>
+          <t>ADIDAS MATCH 3.3 BLACK LIME 2024</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SKU: 32439-P</t>
+          <t>SKU: 110138-P</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/bullpadel-indiga-w-mujer-2023-32439-p</t>
+          <t>https://www.padelnuestro.com/adidas-match-3-3-black-lime-2024-110138-p</t>
         </is>
       </c>
     </row>
@@ -1106,12 +1106,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ADIDAS MATCH 3.3 BLACK LIME 2024</t>
+          <t>BULLPADEL INDIGA CTR 2024</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SKU: 110138-P</t>
+          <t>SKU: 32438-P</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1121,41 +1121,41 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-match-3-3-black-lime-2024-110138-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-indiga-ctr-2024-32438-p</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BULLPADEL INDIGA CTR 2024</t>
+          <t>BLACK CROWN WOLF</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SKU: 32438-P</t>
+          <t>SKU: 19745-P</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>52,95 €</t>
+          <t>54,95 €</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/bullpadel-indiga-ctr-2024-32438-p</t>
+          <t>https://www.padelnuestro.com/black-crown-wolf-19745-p</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BLACK CROWN WOLF</t>
+          <t>DUNLOP SPEED ELITE HL</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SKU: 19745-P</t>
+          <t>SKU: 24777-P</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1165,41 +1165,41 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-wolf-19745-p</t>
+          <t>https://www.padelnuestro.com/dunlop-speed-elite-hl-24777-p</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>DUNLOP SPEED ELITE HL</t>
+          <t>DUNLOP ROCKET TOUR ROJO</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SKU: 24777-P</t>
+          <t>SKU: 104761-P</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>54,95 €</t>
+          <t>55,95 €</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-speed-elite-hl-24777-p</t>
+          <t>https://www.padelnuestro.com/dunlop-rocket-tour-rojo-104761-p</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>DUNLOP ROCKET TOUR ROJO</t>
+          <t>ENEBE NITRO GREEN JUNIOR 2024</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SKU: 104761-P</t>
+          <t>SKU: 111893-P</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1209,19 +1209,19 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-rocket-tour-rojo-104761-p</t>
+          <t>https://www.padelnuestro.com/enebe-response-fiber-blue-111893-p</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ENEBE NITRO GREEN JUNIOR 2024</t>
+          <t>ENEBE NITRO RED JUNIOR</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SKU: 111893-P</t>
+          <t>SKU: 111895-P</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1231,51 +1231,51 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-response-fiber-blue-111893-p</t>
+          <t>https://www.padelnuestro.com/black-crown-piton-air-12k-24-111895-p</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ENEBE NITRO RED JUNIOR</t>
+          <t>NOX SILHOUTTE CASUAL SERIES 23</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SKU: 111895-P</t>
+          <t>SKU: 31591-P</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>55,95 €</t>
+          <t>58,95 €</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-piton-air-12k-24-111895-p</t>
+          <t>https://www.padelnuestro.com/nox-silhoutte-casual-series-23-31591-p</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>NOX SILHOUTTE CASUAL SERIES 23</t>
+          <t>ADIDAS ADIPOWER JUNIOR 3.3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SKU: 31591-P</t>
+          <t>SKU: 110127-P</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>58,95 €</t>
+          <t>59,95 €</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/nox-silhoutte-casual-series-23-31591-p</t>
+          <t>https://www.padelnuestro.com/adidas-adipower-junior-3-3-110127-p</t>
         </is>
       </c>
     </row>
@@ -1326,12 +1326,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ADIDAS ADIPOWER JUNIOR 3.3</t>
+          <t>BULLPADEL HACK 03 JR 2024</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SKU: 110127-P</t>
+          <t>SKU: 110910-P</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1341,19 +1341,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-adipower-junior-3-3-110127-p</t>
+          <t>https://www.padelnuestro.com/siux-genesis-ii-lucho-capra-pro-110910-p</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BULLPADEL HACK 03 JR 2024</t>
+          <t>WILSON BELA V2 KID</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SKU: 110910-P</t>
+          <t>SKU: 105140-P</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1363,19 +1363,19 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-genesis-ii-lucho-capra-pro-110910-p</t>
+          <t>https://www.padelnuestro.com/wilson-bela-v2-kid-105140-p</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>STARVIE JUNIOR 2024</t>
+          <t>ENEBE NITRO RED 2024</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SKU: 112020-P</t>
+          <t>SKU: 111894-P</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1385,19 +1385,19 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/starvie-junior-2024-112020-p</t>
+          <t>https://www.padelnuestro.com/enebe-response-fiber-purple-111894-p</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>WILSON BELA V2 KID</t>
+          <t>ENEBE NITRO GREEN 2024</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SKU: 105140-P</t>
+          <t>SKU: 111892-P</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1407,19 +1407,19 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/wilson-bela-v2-kid-105140-p</t>
+          <t>https://www.padelnuestro.com/enebe-nitro-red-junior-111892-p</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ENEBE NITRO RED 2024</t>
+          <t>STARVIE JUNIOR 2024</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SKU: 111894-P</t>
+          <t>SKU: 112020-P</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1429,19 +1429,19 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-response-fiber-purple-111894-p</t>
+          <t>https://www.padelnuestro.com/starvie-junior-2024-112020-p</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ENEBE NITRO GREEN 2024</t>
+          <t>BABOLAT CONTACT 2022</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SKU: 111892-P</t>
+          <t>SKU: 29149-P</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1451,19 +1451,19 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-nitro-red-junior-111892-p</t>
+          <t>https://www.padelnuestro.com/babolat-contact-2022-29149-p</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>HARLEM HELIX</t>
+          <t>BABOLAT REVEAL 2022</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SKU: 30326-P</t>
+          <t>SKU: 29150-P</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1473,19 +1473,19 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/harlem-helix-30326-p</t>
+          <t>https://www.padelnuestro.com/babolat-reveal-2022-29150-p</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BABOLAT CONTACT 2022</t>
+          <t>HARLEM HELIX</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SKU: 29149-P</t>
+          <t>SKU: 30326-P</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1495,19 +1495,19 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/babolat-contact-2022-29149-p</t>
+          <t>https://www.padelnuestro.com/harlem-helix-30326-p</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BABOLAT REVEAL 2022</t>
+          <t>SIUX ASTRA 3.0 HYBRID</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SKU: 29150-P</t>
+          <t>SKU: 28766-P</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1517,19 +1517,19 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/babolat-reveal-2022-29150-p</t>
+          <t>https://www.padelnuestro.com/siux-astra-3-0-hybrid-28766-p</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>SIUX ASTRA 3.0 HYBRID</t>
+          <t>SIUX SX7 AIR</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SKU: 28766-P</t>
+          <t>SKU: 28786-P</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1539,19 +1539,19 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-astra-3-0-hybrid-28766-p</t>
+          <t>https://www.padelnuestro.com/siux-sx7-air-28786-p</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SIUX SX7 AIR</t>
+          <t>NOX X-ONE EVO RED</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SKU: 28786-P</t>
+          <t>SKU: 31590-P</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1561,19 +1561,19 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-sx7-air-28786-p</t>
+          <t>https://www.padelnuestro.com/nox-x-one-evo-red-31590-p</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BULLPADEL RAIDER CONTROL</t>
+          <t>ADIDAS DRIVE LIGHT 3.3</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SKU: 21725-P</t>
+          <t>SKU: 110137-P</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/bullpadel-raider-control-21725-p</t>
+          <t>https://www.padelnuestro.com/adidas-drive-light-3-3-110137-p</t>
         </is>
       </c>
     </row>
@@ -1612,12 +1612,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>NOX X-ONE EVO RED</t>
+          <t>BULLPADEL RAIDER CONTROL</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SKU: 31590-P</t>
+          <t>SKU: 21725-P</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1627,151 +1627,151 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/nox-x-one-evo-red-31590-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-raider-control-21725-p</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ADIDAS DRIVE LIGHT 3.3</t>
+          <t>HEAD CHALLENGE AZUL VERDE</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>SKU: 110137-P</t>
+          <t>SKU: 24991-P</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>59,95 €</t>
+          <t>61,95 €</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-drive-light-3-3-110137-p</t>
+          <t>https://www.padelnuestro.com/head-challenge-azul-verde-24991-p</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>HEAD EVO EXTREME 2023</t>
+          <t>DUNLOP RAPID CONTROL 4.0</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>SKU: 110099-P</t>
+          <t>SKU: 104758-P</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>60,95 €</t>
+          <t>62,95 €</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-evo-extreme-2023-110099-p</t>
+          <t>https://www.padelnuestro.com/dunlop-rapid-control-4-0-104758-p</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HEAD CHALLENGE AZUL VERDE</t>
+          <t>ADIDAS DRIVE 3.3 VINTAGE</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>SKU: 24991-P</t>
+          <t>SKU: 110136-P</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>61,95 €</t>
+          <t>63,95 €</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-challenge-azul-verde-24991-p</t>
+          <t>https://www.padelnuestro.com/adidas-drive-3-3-vintage-110136-p</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DUNLOP RAPID CONTROL 4.0</t>
+          <t>ENEBE COMBAT ULTRASOFT CELESTE</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SKU: 104758-P</t>
+          <t>SKU: 24675-P</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>62,95 €</t>
+          <t>63,95 €</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-rapid-control-4-0-104758-p</t>
+          <t>https://www.padelnuestro.com/enebe-combat-ultrasoft-celeste-24675-p</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ADIDAS DRIVE 3.3 VINTAGE</t>
+          <t>VAIRO ACROSS PINK</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>SKU: 110136-P</t>
+          <t>SKU: 105771-P</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>63,95 €</t>
+          <t>64,95 €</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-drive-3-3-vintage-110136-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-pink-105771-p</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>ENEBE COMBAT ULTRASOFT CELESTE</t>
+          <t>NOX AT10 GENIUS ULTRALIGHT 23</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>SKU: 24675-P</t>
+          <t>SKU: 31593-P</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>63,95 €</t>
+          <t>64,95 €</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-combat-ultrasoft-celeste-24675-p</t>
+          <t>https://www.padelnuestro.com/nox-at10-genius-ultralight-23-31593-p</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS PINK</t>
+          <t>VAIRO ACROSS ORANGE</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>SKU: 105771-P</t>
+          <t>SKU: 105770-P</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1781,19 +1781,19 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-pink-105771-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-orange-105770-p</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>NOX AT10 GENIUS ULTRALIGHT 23</t>
+          <t>VAIRO ACROSS YELLOW</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SKU: 31593-P</t>
+          <t>SKU: 105772-P</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1803,19 +1803,19 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/nox-at10-genius-ultralight-23-31593-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-yellow-105772-p</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS ORANGE</t>
+          <t>VAIRO ACROSS ORANGE SAND FINISH</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>SKU: 105770-P</t>
+          <t>SKU: 106606-P</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1825,19 +1825,19 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-orange-105770-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-orange-sand-finish-106606-p</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS YELLOW</t>
+          <t>VAIRO ACROSS PINK SAND FINISH</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>SKU: 105772-P</t>
+          <t>SKU: 106607-P</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1847,19 +1847,19 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-yellow-105772-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-pink-sand-finish-106607-p</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS ORANGE SAND FINISH</t>
+          <t>VAIRO ACROSS YELLOW SAND FINISH</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>SKU: 106606-P</t>
+          <t>SKU: 106608-P</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1869,19 +1869,19 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-orange-sand-finish-106606-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-yellow-sand-finish-106608-p</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS PINK SAND FINISH</t>
+          <t>VAIRO ACROSS BLUE SAND FINISH</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>SKU: 106607-P</t>
+          <t>SKU: 106605-P</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1891,19 +1891,19 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-pink-sand-finish-106607-p</t>
+          <t>https://www.padelnuestro.com/vairo-across-blue-sand-finish-106605-p</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS YELLOW SAND FINISH</t>
+          <t>VIBOR-A TITAN JUNIOR CLASSIC FIBER 2024</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>SKU: 106608-P</t>
+          <t>SKU: 111915-P</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1913,239 +1913,239 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-yellow-sand-finish-106608-p</t>
+          <t>https://www.padelnuestro.com/vibor-a-titan-junior-classic-fiber-2024-111915-p</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>VAIRO ACROSS BLUE SAND FINISH</t>
+          <t>DUNLOP RAPID POWER 4.0</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>SKU: 106605-P</t>
+          <t>SKU: 104759-P</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>64,95 €</t>
+          <t>65,95 €</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vairo-across-blue-sand-finish-106605-p</t>
+          <t>https://www.padelnuestro.com/dunlop-rapid-power-4-0-104759-p</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>VIBOR-A TITAN JUNIOR CLASSIC FIBER 2024</t>
+          <t>STARVIE ARCADIA 2024</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>SKU: 111915-P</t>
+          <t>SKU: 112008-P</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>64,95 €</t>
+          <t>66,95 €</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vibor-a-titan-junior-classic-fiber-2024-111915-p</t>
+          <t>https://www.padelnuestro.com/starvie-arcadia-2024-112008-p</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BULLPADEL BUKET X SERIES</t>
+          <t>HEAD MONSTER KIDS</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SKU: 29614-P</t>
+          <t>SKU: 112549-P</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>64,95 €</t>
+          <t>67,95 €</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/pn-29614-p</t>
+          <t>https://www.padelnuestro.com/head-monster-kids-112549-p</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>DUNLOP RAPID POWER 4.0</t>
+          <t>BLACK CROWN SHARK</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>SKU: 104759-P</t>
+          <t>SKU: 19744-P</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>65,95 €</t>
+          <t>67,95 €</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-rapid-power-4-0-104759-p</t>
+          <t>https://www.padelnuestro.com/black-crown-shark-19744-p</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>STARVIE ARCADIA 2024</t>
+          <t>HEAD EXTREME JUNIOR 2023</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SKU: 112008-P</t>
+          <t>SKU: 110101-P</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>66,95 €</t>
+          <t>68,95 €</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/starvie-arcadia-2024-112008-p</t>
+          <t>https://www.padelnuestro.com/head-extreme-junior-2023-110101-p</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>HEAD MONSTER KIDS</t>
+          <t>SIUX BEAT KID</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SKU: 112549-P</t>
+          <t>SKU: 109592-P</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>67,95 €</t>
+          <t>68,99 €</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-monster-kids-112549-p</t>
+          <t>https://www.padelnuestro.com/babolat-counter-viper-2024-109592-p</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>BLACK CROWN SHARK</t>
+          <t>ADIDAS METALBONE YOUTH 3.2 JUNIOR 2023</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>SKU: 19744-P</t>
+          <t>SKU: 32317-P</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>67,95 €</t>
+          <t>69,00 €</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-shark-19744-p</t>
+          <t>https://www.padelnuestro.com/adidas-metalbone-youth-3-2-junior-2023-32317-p</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>HEAD EXTREME JUNIOR 2023</t>
+          <t>SOFTEE RAZE EVOLUTION ORANGE CARBONO</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SKU: 110101-P</t>
+          <t>SKU: 112484-P</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>68,95 €</t>
+          <t>69,95 €</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-extreme-junior-2023-110101-p</t>
+          <t>https://www.padelnuestro.com/softee-raze-evolution-orange-carbono-112484-p</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>SIUX BEAT KID</t>
+          <t>SIUX DIABLO REVOLUTION JR 3</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SKU: 109592-P</t>
+          <t>SKU: 109471-P</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>68,99 €</t>
+          <t>69,95 €</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/babolat-counter-viper-2024-109592-p</t>
+          <t>https://www.padelnuestro.com/siux-diablo-revolution-jr-3-109471-p</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ADIDAS METALBONE YOUTH 3.2 JUNIOR 2023</t>
+          <t>SIUX ELECTRA JR ST3</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SKU: 32317-P</t>
+          <t>SKU: 109475-P</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>69,00 €</t>
+          <t>69,95 €</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-metalbone-youth-3-2-junior-2023-32317-p</t>
+          <t>https://www.padelnuestro.com/siux-electra-jr-st3-109475-p</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>DUNLOP IMPACT CARBON PRO LTD NARANJA</t>
+          <t>BLACK CROWN SNAKE 2022</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SKU: 31559-P</t>
+          <t>SKU: 26422-P</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2155,19 +2155,19 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-naranja-31559-p</t>
+          <t>https://www.padelnuestro.com/black-crown-snake-2022-26422-p</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>SIUX ELECTRA JR ST3</t>
+          <t>DUNLOP IMPACT CARBON PRO LTD NARANJA</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>SKU: 109475-P</t>
+          <t>SKU: 31559-P</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2177,19 +2177,19 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-electra-jr-st3-109475-p</t>
+          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-naranja-31559-p</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>SOFTEE RAZE EVOLUTION ORANGE CARBONO</t>
+          <t>DUNLOP IMPACT CARBON PRO LTD AZUL</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>SKU: 112484-P</t>
+          <t>SKU: 107264-P</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2199,19 +2199,19 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/softee-raze-evolution-orange-carbono-112484-p</t>
+          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-azul-107264-p</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>BLACK CROWN SNAKE 2022</t>
+          <t>HEAD ULTIMATE POWER YELLOW WITH CB</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SKU: 26422-P</t>
+          <t>SKU: 29566-P</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2221,19 +2221,19 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-snake-2022-26422-p</t>
+          <t>https://www.padelnuestro.com/head-ultimate-power-yellow-with-cb-29566-p</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>SIUX DIABLO REVOLUTION JR 3</t>
+          <t>BULLPADEL FLOW LIGHT MUJER 2024</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SKU: 109471-P</t>
+          <t>SKU: 32436-P</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2243,19 +2243,19 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-diablo-revolution-jr-3-109471-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-flow-light-mujer-2024-32436-p</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>HEAD ULTIMATE POWER YELLOW WITH CB</t>
+          <t>ADIDAS RX SERIES LIME 2024</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>SKU: 29566-P</t>
+          <t>SKU: 110150-P</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2265,19 +2265,19 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-ultimate-power-yellow-with-cb-29566-p</t>
+          <t>https://www.padelnuestro.com/adidas-rx-series-lime-2024-110150-p</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>DUNLOP IMPACT CARBON PRO LTD AZUL</t>
+          <t>STAR VIE VESTA</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>SKU: 107264-P</t>
+          <t>SKU: 21832-P</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2287,19 +2287,19 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-azul-107264-p</t>
+          <t>https://www.padelnuestro.com/star-vie-vesta-21832-p</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>BULLPADEL FLOW LIGHT MUJER 2024</t>
+          <t>DUNLOP IMPACT CARBON PRO LTD BLK</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>SKU: 32436-P</t>
+          <t>SKU: 31557-P</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2309,19 +2309,19 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/bullpadel-flow-light-mujer-2024-32436-p</t>
+          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-blk-31557-p</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>STAR VIE VESTA</t>
+          <t>DUNLOP IMPACT CARBON PRO LTD AMARILLA</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>SKU: 21832-P</t>
+          <t>SKU: 31558-P</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2331,19 +2331,19 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/star-vie-vesta-21832-p</t>
+          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-amarilla-31558-p</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DUNLOP IMPACT CARBON PRO LTD BLK</t>
+          <t>DUNLOP IMPACT CARBON PRO LTD WOMAN</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>SKU: 31557-P</t>
+          <t>SKU: 31560-P</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2353,129 +2353,129 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-blk-31557-p</t>
+          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-woman-31560-p</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>DUNLOP IMPACT CARBON PRO LTD AMARILLA</t>
+          <t>ENEBE CROSS</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>SKU: 31558-P</t>
+          <t>SKU: 29285-P</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>69,95 €</t>
+          <t>70,95 €</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-amarilla-31558-p</t>
+          <t>https://www.padelnuestro.com/enebe-cross-29285-p</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>DUNLOP IMPACT CARBON PRO LTD WOMAN</t>
+          <t>ADIDAS RX SERIES RED 2024</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SKU: 31560-P</t>
+          <t>SKU: 110151-P</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>69,95 €</t>
+          <t>71,95 €</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-impact-carbon-pro-ltd-woman-31560-p</t>
+          <t>https://www.padelnuestro.com/adidas-rx-series-red-2024-110151-p</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>ADIDAS RX SERIES LIME 2024</t>
+          <t>BABOLAT STORM 2022</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>SKU: 110150-P</t>
+          <t>SKU: 29148-P</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>69,95 €</t>
+          <t>74,95 €</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-rx-series-lime-2024-110150-p</t>
+          <t>https://www.padelnuestro.com/babolat-storm-2022-29148-p</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ENEBE CROSS</t>
+          <t>BULLPADEL BP10 EVO 2024</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>SKU: 29285-P</t>
+          <t>SKU: 32435-P</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>70,95 €</t>
+          <t>74,95 €</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-cross-29285-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-bp10-evo-2024-32435-p</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ADIDAS RX SERIES RED 2024</t>
+          <t>SIUX EVOQUE 3 AIR</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>SKU: 110151-P</t>
+          <t>SKU: 28780-P</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>71,95 €</t>
+          <t>74,95 €</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-rx-series-red-2024-110151-p</t>
+          <t>https://www.padelnuestro.com/siux-evoque-3-air-28780-p</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>BULLPADEL BP10 EVO 2024</t>
+          <t>HEAD ULTIMATE POWER II WITH CB AMARILLO VERDE</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>SKU: 32435-P</t>
+          <t>SKU: 29568-P</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2485,19 +2485,19 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/bullpadel-bp10-evo-2024-32435-p</t>
+          <t>https://www.padelnuestro.com/head-ultimate-power-ii-with-cb-amarillo-verde-29568-p</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>BABOLAT STORM 2022</t>
+          <t>BULLPADEL BRAVE 3.0</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>SKU: 29148-P</t>
+          <t>SKU: 24564-P</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2507,19 +2507,19 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/babolat-storm-2022-29148-p</t>
+          <t>https://www.padelnuestro.com/bullpadel-brave-3-0-24564-p</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>SIUX EVOQUE 3 AIR</t>
+          <t>HEAD ULTIMATE POWER II WITH CB NARANJA</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>SKU: 28780-P</t>
+          <t>SKU: 29569-P</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2529,129 +2529,129 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-evoque-3-air-28780-p</t>
+          <t>https://www.padelnuestro.com/head-ultimate-power-ii-with-cb-naranja-29569-p</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>BULLPADEL BRAVE 3.0</t>
+          <t>SOFTEE RAZE EVOLUTION GREEN CARBONO</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>SKU: 24564-P</t>
+          <t>SKU: 112483-P</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>74,95 €</t>
+          <t>75,95 €</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/bullpadel-brave-3-0-24564-p</t>
+          <t>https://www.padelnuestro.com/softee-raze-evolution-green-carbono-112483-p</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>HEAD ULTIMATE POWER II WITH CB AMARILLO VERDE</t>
+          <t>STARVIE VESTA 2024</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>SKU: 29568-P</t>
+          <t>SKU: 112028-P</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>74,95 €</t>
+          <t>76,95 €</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-ultimate-power-ii-with-cb-amarillo-verde-29568-p</t>
+          <t>https://www.padelnuestro.com/starvie-vesta-2024-112028-p</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>HEAD ULTIMATE POWER II WITH CB NARANJA</t>
+          <t>SIUX INFERNAL AVANT</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>SKU: 29569-P</t>
+          <t>SKU: 24351-P</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>74,95 €</t>
+          <t>79,00 €</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/head-ultimate-power-ii-with-cb-naranja-29569-p</t>
+          <t>https://www.padelnuestro.com/siux-infernal-avant-24351-p</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>SOFTEE RAZE EVOLUTION GREEN CARBONO</t>
+          <t>SIUX BEAT HYBRID AIR</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SKU: 112483-P</t>
+          <t>SKU: 109469-P</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>75,95 €</t>
+          <t>79,00 €</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/softee-raze-evolution-green-carbono-112483-p</t>
+          <t>https://www.padelnuestro.com/siux-beat-hybrid-air-109469-p</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>STARVIE VESTA 2024</t>
+          <t>SIUX TITANIA LADY 2.0</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>SKU: 112028-P</t>
+          <t>SKU: 25185-P</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>76,95 €</t>
+          <t>79,00 €</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/starvie-vesta-2024-112028-p</t>
+          <t>https://www.padelnuestro.com/wilson-carbon-force-pro-padel-2-25185-p</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>SIUX INFERNAL AVANT</t>
+          <t>SIUX BEAT CONTROL</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>SKU: 24351-P</t>
+          <t>SKU: 109467-P</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2661,19 +2661,19 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-infernal-avant-24351-p</t>
+          <t>https://www.padelnuestro.com/siux-beat-control-109467-p</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>SIUX TITANIA LADY 2.0</t>
+          <t>SIUX BEAT HYBRID</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SKU: 25185-P</t>
+          <t>SKU: 109468-P</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2683,85 +2683,85 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/wilson-carbon-force-pro-padel-2-25185-p</t>
+          <t>https://www.padelnuestro.com/siux-beat-hybrid-109468-p</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>SIUX BEAT HYBRID AIR</t>
+          <t>DUNLOP NEMESIS CONTROL</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>SKU: 109469-P</t>
+          <t>SKU: 31550-P</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>79,00 €</t>
+          <t>79,95 €</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-beat-hybrid-air-109469-p</t>
+          <t>https://www.padelnuestro.com/dunlop-nemesis-control-31550-p</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>SIUX BEAT CONTROL</t>
+          <t>DUNLOP GRAVITY</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>SKU: 109467-P</t>
+          <t>SKU: 31553-P</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>79,00 €</t>
+          <t>79,95 €</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-beat-control-109467-p</t>
+          <t>https://www.padelnuestro.com/dunlop-gravity-31553-p</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>SIUX BEAT HYBRID</t>
+          <t>DUNLOP INFERNO GOLD</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>SKU: 109468-P</t>
+          <t>SKU: 26379-P</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>79,00 €</t>
+          <t>79,95 €</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/siux-beat-hybrid-109468-p</t>
+          <t>https://www.padelnuestro.com/dunlop-inferno-gold-26379-p</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>DUNLOP NEMESIS CONTROL</t>
+          <t>DUNLOP NEMESIS</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>SKU: 31550-P</t>
+          <t>SKU: 31552-P</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2771,19 +2771,19 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-nemesis-control-31550-p</t>
+          <t>https://www.padelnuestro.com/dunlop-nemesis-31552-p</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>DUNLOP GRAVITY</t>
+          <t>DUNLOP GALAXY</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SKU: 31553-P</t>
+          <t>SKU: 31554-P</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2793,293 +2793,293 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-gravity-31553-p</t>
+          <t>https://www.padelnuestro.com/dunlop-galaxy-31554-p</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>DUNLOP INFERNO GOLD</t>
+          <t>ADIDAS RX SERIES LIGHT 2024</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SKU: 26379-P</t>
+          <t>SKU: 110149-P</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>79,95 €</t>
+          <t>81,95 €</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-inferno-gold-26379-p</t>
+          <t>https://www.padelnuestro.com/adidas-rx-series-light-2024-110149-p</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>DUNLOP NEMESIS</t>
+          <t>PRINCE AIR V</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>SKU: 31552-P</t>
+          <t>SKU: 109953-P</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>79,95 €</t>
+          <t>81,95 €</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-nemesis-31552-p</t>
+          <t>https://www.padelnuestro.com/babolat-technical-veron-2024-109953-p</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>DUNLOP GALAXY</t>
+          <t>VIBOR-A BELCHER CLASSIC FIBER 2024</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SKU: 31554-P</t>
+          <t>SKU: 111905-P</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>79,95 €</t>
+          <t>82,95 €</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/dunlop-galaxy-31554-p</t>
+          <t>https://www.padelnuestro.com/vibor-a-belcher-classic-fiber-2024-111905-p</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>ADIDAS RX SERIES LIGHT 2024</t>
+          <t>ENEBE RS 9.1 ORANGE 2024</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>SKU: 110149-P</t>
+          <t>SKU: 111901-P</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81,95 €</t>
+          <t>82,95 €</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-rx-series-light-2024-110149-p</t>
+          <t>https://www.padelnuestro.com/enebe-rs-9-1-orange-2024-111901-p</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>PRINCE AIR V</t>
+          <t>NOX EQUATION ADVANCED SERIES 2024</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>SKU: 109953-P</t>
+          <t>SKU: 110806-P</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81,95 €</t>
+          <t>83,95 €</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/babolat-technical-veron-2024-109953-p</t>
+          <t>https://www.padelnuestro.com/nox-equation-advanced-series-2024-110806-p</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>VIBOR-A BELCHER CLASSIC FIBER 2024</t>
+          <t>SOFTEE BLOQUER 2024</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>SKU: 111905-P</t>
+          <t>SKU: 112475-P</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>82,95 €</t>
+          <t>83,95 €</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/vibor-a-belcher-classic-fiber-2024-111905-p</t>
+          <t>https://www.padelnuestro.com/softee-bloquer-2024-112475-p</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>ENEBE RS 9.1 ORANGE 2024</t>
+          <t>ADIDAS METALBONE YOUTH 3.3 2024</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>SKU: 111901-P</t>
+          <t>SKU: 110148-P</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>82,95 €</t>
+          <t>84,95 €</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-rs-9-1-orange-2024-111901-p</t>
+          <t>https://www.padelnuestro.com/adidas-metalbone-youth-3-3-2024-110148-p</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>SOFTEE BLOQUER 2024</t>
+          <t>BLACK CROWN PITON NAKANO</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>SKU: 112475-P</t>
+          <t>SKU: 18189-P</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>83,95 €</t>
+          <t>84,95 €</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/softee-bloquer-2024-112475-p</t>
+          <t>https://www.padelnuestro.com/black-crown-piton-nakano-18189-p</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>NOX EQUATION ADVANCED SERIES 2024</t>
+          <t>BLACK CROWN HURRICANE 2022</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>SKU: 110806-P</t>
+          <t>SKU: 26421-P</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>83,95 €</t>
+          <t>85,95 €</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/nox-equation-advanced-series-2024-110806-p</t>
+          <t>https://www.padelnuestro.com/black-crown-hurricane-2022-26421-p</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>ADIDAS METALBONE YOUTH 3.3 2024</t>
+          <t>ENEBE RS 9.1 BLUE 2024</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SKU: 110148-P</t>
+          <t>SKU: 111900-P</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>84,95 €</t>
+          <t>87,95 €</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/adidas-metalbone-youth-3-3-2024-110148-p</t>
+          <t>https://www.padelnuestro.com/enebe-rs-9-1-blue-2024-111900-p</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>BLACK CROWN PITON NAKANO</t>
+          <t>HEAD ZEPHYR 2023</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>SKU: 18189-P</t>
+          <t>SKU: 32515-P</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>84,95 €</t>
+          <t>88,00 €</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-piton-nakano-18189-p</t>
+          <t>https://www.padelnuestro.com/head-zephyr-2023-32515-p</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>BLACK CROWN HURRICANE 2022</t>
+          <t>HEAD ZEPHYR 2023</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>SKU: 26421-P</t>
+          <t>SKU: 113579-P</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>85,95 €</t>
+          <t>88,00 €</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/black-crown-hurricane-2022-26421-p</t>
+          <t>https://www.padelnuestro.com/head-zephyr-2023-113579-p</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>ENEBE RS 9.1 BLUE 2024</t>
+          <t>DUNLOP TITAN 2.0 AMARILLA AZUL</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>SKU: 111900-P</t>
+          <t>SKU: 110872-P</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>87,95 €</t>
+          <t>89,95 €</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>https://www.padelnuestro.com/enebe-rs-9-1-blue-2024-111900-p</t>
+          <t>https://www.padelnuestro.com/dunlop-titan-killer-2-0-2024-110872-p</t>
         </is>
       </c>
     </row>

</xml_diff>